<commit_message>
doesnt add bazacalcul if already exists
</commit_message>
<xml_diff>
--- a/macheta.xlsx
+++ b/macheta.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\munca\webapp-spring\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="9120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="9120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="date factura" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -141,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,7 +335,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +370,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -552,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -562,33 +557,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="12"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>33</v>
       </c>
@@ -597,12 +592,12 @@
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -611,14 +606,14 @@
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -627,28 +622,28 @@
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -659,21 +654,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -681,7 +676,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
@@ -690,156 +685,156 @@
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -858,27 +853,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
-    <col min="18" max="20" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" customWidth="1"/>
+    <col min="18" max="20" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -892,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -952,7 +947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M3" t="s">
         <v>4</v>
       </c>

</xml_diff>